<commit_message>
Updated documentation for sprint 4 review Added the sprint 4 backlog and the use case scenario for librarians viewing member details/history
</commit_message>
<xml_diff>
--- a/sprints/Sprint 4/Sprint4Backlog.xlsx
+++ b/sprints/Sprint 4/Sprint4Backlog.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2D5CC7-D0AC-4247-BB0A-DB8C150EDAE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,15 +19,92 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+  <si>
+    <t>Progress</t>
+  </si>
+  <si>
+    <t>Assignee</t>
+  </si>
+  <si>
+    <t>User Role</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>ETA</t>
+  </si>
+  <si>
+    <t>DEADLINE</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Luke</t>
+  </si>
+  <si>
+    <t>Tristen</t>
+  </si>
+  <si>
+    <t>Carson</t>
+  </si>
+  <si>
+    <t>Luke/Tristen/Carson</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>Member</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warehouse employee </t>
+  </si>
+  <si>
+    <t>Librarian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Turn records of items tracked by employees into a table on the desktop app </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Be able to remove and update addresses </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add ability to flag for damaged returns </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement view for librarians  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">implement view for viewing users history/information </t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -49,8 +127,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +411,136 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="3">
+        <v>43900</v>
+      </c>
+      <c r="F2" s="3">
+        <v>43901</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="3">
+        <v>43900</v>
+      </c>
+      <c r="F3" s="3">
+        <v>43901</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="3">
+        <v>43900</v>
+      </c>
+      <c r="F4" s="3">
+        <v>43901</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="3">
+        <v>43900</v>
+      </c>
+      <c r="F5" s="3">
+        <v>43901</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="3">
+        <v>43900</v>
+      </c>
+      <c r="F6" s="3">
+        <v>43901</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated documentation Updated the sprint 4 backlog to match Dr. Corleys sprint review comments. Put all use case scenariors in one folder removing the sub folders for each sprint.
</commit_message>
<xml_diff>
--- a/sprints/Sprint 4/Sprint4Backlog.xlsx
+++ b/sprints/Sprint 4/Sprint4Backlog.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2D5CC7-D0AC-4247-BB0A-DB8C150EDAE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0822F1C-AB14-4D6E-8072-17F5CD7B268F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
   <si>
     <t>Progress</t>
   </si>
@@ -70,16 +70,40 @@
     <t xml:space="preserve">Turn records of items tracked by employees into a table on the desktop app </t>
   </si>
   <si>
-    <t xml:space="preserve">Be able to remove and update addresses </t>
-  </si>
-  <si>
     <t xml:space="preserve">Add ability to flag for damaged returns </t>
   </si>
   <si>
     <t xml:space="preserve">Implement view for librarians  </t>
   </si>
   <si>
-    <t xml:space="preserve">implement view for viewing users history/information </t>
+    <t xml:space="preserve">Implement functionality to remove addresses </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement DB call to remove addresses (flag as not in use, but keep in DB for record purpose) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add functionality to DB for flagging rentals </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement view for viewing users history/information </t>
+  </si>
+  <si>
+    <t>Implement librarian table in the DB for logging in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement ability to filter members by who is overdue </t>
+  </si>
+  <si>
+    <t>Estimation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 day </t>
+  </si>
+  <si>
+    <t>2 days</t>
+  </si>
+  <si>
+    <t>1 day</t>
   </si>
 </sst>
 </file>
@@ -412,15 +436,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -439,8 +463,11 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -459,8 +486,11 @@
       <c r="F2" s="3">
         <v>43901</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -471,73 +501,177 @@
         <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="3">
+        <v>43900</v>
+      </c>
+      <c r="F3" s="3">
+        <v>43901</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="3">
+        <v>43900</v>
+      </c>
+      <c r="F4" s="3">
+        <v>43901</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="3">
-        <v>43900</v>
-      </c>
-      <c r="F3" s="3">
-        <v>43901</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="E5" s="3">
+        <v>43900</v>
+      </c>
+      <c r="F5" s="3">
+        <v>43901</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="3">
+        <v>43900</v>
+      </c>
+      <c r="F6" s="3">
+        <v>43901</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="3">
-        <v>43900</v>
-      </c>
-      <c r="F4" s="3">
-        <v>43901</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="E7" s="3">
+        <v>43900</v>
+      </c>
+      <c r="F7" s="3">
+        <v>43901</v>
+      </c>
+      <c r="G7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C8" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="3">
-        <v>43900</v>
-      </c>
-      <c r="F5" s="3">
-        <v>43901</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="D8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="3">
+        <v>43900</v>
+      </c>
+      <c r="F8" s="3">
+        <v>43901</v>
+      </c>
+      <c r="G8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C9" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="3">
-        <v>43900</v>
-      </c>
-      <c r="F6" s="3">
-        <v>43901</v>
+      <c r="D9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="3">
+        <v>43900</v>
+      </c>
+      <c r="F9" s="3">
+        <v>43901</v>
+      </c>
+      <c r="G9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="3">
+        <v>43900</v>
+      </c>
+      <c r="F10" s="3">
+        <v>43901</v>
+      </c>
+      <c r="G10" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Backlog Completion Check. Updated backlog. Went through all the projects to ensure that all features from the current sprint backlog were complete
</commit_message>
<xml_diff>
--- a/sprints/Sprint 4/Sprint4Backlog.xlsx
+++ b/sprints/Sprint 4/Sprint4Backlog.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0822F1C-AB14-4D6E-8072-17F5CD7B268F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7936F2C-830C-4C9A-8158-3E5F1D820026}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,9 +40,6 @@
     <t>DEADLINE</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>Luke</t>
   </si>
   <si>
@@ -104,6 +101,9 @@
   </si>
   <si>
     <t>1 day</t>
+  </si>
+  <si>
+    <t>Complete</t>
   </si>
 </sst>
 </file>
@@ -439,10 +439,14 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="4" max="4" width="82.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -464,21 +468,21 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" s="3">
         <v>43900</v>
@@ -487,21 +491,21 @@
         <v>43901</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" s="3">
         <v>43900</v>
@@ -510,21 +514,21 @@
         <v>43901</v>
       </c>
       <c r="G3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4" s="3">
         <v>43900</v>
@@ -533,21 +537,21 @@
         <v>43901</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="3">
         <v>43900</v>
@@ -556,21 +560,21 @@
         <v>43901</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" s="3">
         <v>43900</v>
@@ -579,21 +583,21 @@
         <v>43901</v>
       </c>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7" s="3">
         <v>43900</v>
@@ -602,21 +606,21 @@
         <v>43901</v>
       </c>
       <c r="G7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8" s="3">
         <v>43900</v>
@@ -625,21 +629,21 @@
         <v>43901</v>
       </c>
       <c r="G8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E9" s="3">
         <v>43900</v>
@@ -648,21 +652,21 @@
         <v>43901</v>
       </c>
       <c r="G9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E10" s="3">
         <v>43900</v>
@@ -671,7 +675,7 @@
         <v>43901</v>
       </c>
       <c r="G10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>